<commit_message>
add other excel access functions
</commit_message>
<xml_diff>
--- a/xls/1.xlsx
+++ b/xls/1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" activeTab="1"/>
+    <workbookView windowWidth="24045" windowHeight="12375" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>A1</t>
   </si>
@@ -137,6 +137,39 @@
   </si>
   <si>
     <t>C12</t>
+  </si>
+  <si>
+    <t>园区项目</t>
+  </si>
+  <si>
+    <t>门禁设备数</t>
+  </si>
+  <si>
+    <t>道闸设备数</t>
+  </si>
+  <si>
+    <t>视频监控设备数</t>
+  </si>
+  <si>
+    <t>水表设备数</t>
+  </si>
+  <si>
+    <t>电表设备数</t>
+  </si>
+  <si>
+    <t>消防点位</t>
+  </si>
+  <si>
+    <t>消防水泵、风机</t>
+  </si>
+  <si>
+    <t>智造产业园</t>
+  </si>
+  <si>
+    <t>电子电器产业园</t>
+  </si>
+  <si>
+    <t>合计</t>
   </si>
 </sst>
 </file>
@@ -149,13 +182,20 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -307,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +356,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -501,12 +553,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -627,76 +694,70 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -705,10 +766,10 @@
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -717,10 +778,10 @@
     <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -729,10 +790,10 @@
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -741,10 +802,10 @@
     <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -753,15 +814,36 @@
     <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1084,154 +1166,154 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" ht="14.25" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" ht="14.25" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" ht="14.25" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" ht="14.25" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" ht="14.25" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" ht="14.25" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" ht="14.25" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" ht="14.25" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" ht="14.25" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" ht="14.25" spans="1:4">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" ht="14.25" spans="1:4">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" ht="14.25" spans="1:4">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" ht="14.25" spans="1:4">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1245,45 +1327,45 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:3">
-      <c r="A1" s="1">
+    <row r="1" s="6" customFormat="1" spans="1:3">
+      <c r="A1" s="6">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="6">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:3">
-      <c r="A2" s="1">
+    <row r="2" s="6" customFormat="1" spans="1:3">
+      <c r="A2" s="6">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:3">
-      <c r="A3" s="1">
+    <row r="3" s="6" customFormat="1" spans="1:3">
+      <c r="A3" s="6">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>9</v>
       </c>
     </row>
@@ -1297,14 +1379,124 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetData>
+    <row r="1" ht="27" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="3">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1347</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1062</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1148</v>
+      </c>
+      <c r="G2" s="2">
+        <v>53713</v>
+      </c>
+      <c r="H2" s="2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2">
+        <v>76</v>
+      </c>
+      <c r="C3" s="2">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2072</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2156</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2337</v>
+      </c>
+      <c r="G3" s="2">
+        <v>56276</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:H4" si="0">B2+B3</f>
+        <v>128</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>3419</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>3218</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>3485</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>109989</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>